<commit_message>
close #3 string codec内部処理追加
</commit_message>
<xml_diff>
--- a/Samples/cheatsheet.xlsx
+++ b/Samples/cheatsheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="41460" yWindow="1060" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="34180" yWindow="1020" windowWidth="28800" windowHeight="17600" tabRatio="500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="2" r:id="rId1"/>
@@ -54,12 +54,68 @@
             <rFont val="ＭＳ Ｐゴシック"/>
             <charset val="128"/>
           </rPr>
+          <t>"type" : ["string", "null"]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
           <t>"type" : ["string"],
 "required" : true</t>
         </r>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="0">
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : false</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>#1111
+"type" : ["string", "null"],
+# 2222
+"required" : false</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -84,7 +140,32 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office ユーザー</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : true</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -96,36 +177,6 @@
           </rPr>
           <t>"type" : ["string", "null"],
 "required" : false</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="ＭＳ Ｐゴシック"/>
-            <charset val="128"/>
-          </rPr>
-          <t>"type" : ["string", "null"],
-"required" : false</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="ＭＳ Ｐゴシック"/>
-            <charset val="128"/>
-          </rPr>
-          <t>"type" : ["string"],
-"required" : true</t>
         </r>
         <r>
           <rPr>
@@ -136,6 +187,151 @@
           </rPr>
           <t xml:space="preserve">
 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : false</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office ユーザー</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : true</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : false</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : false</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office ユーザー</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : true</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : false</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : false</t>
         </r>
       </text>
     </comment>
@@ -208,188 +404,614 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office ユーザー</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : true</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : false</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : false</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office ユーザー</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : true</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : false</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : false</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office ユーザー</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : true</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : false</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : false</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office ユーザー</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : true</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : false</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : false</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office ユーザー</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : true</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : false</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : false</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office ユーザー</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : true</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : false</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : false</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office ユーザー</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : true</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : false</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <charset val="128"/>
+          </rPr>
+          <t>"type" : ["string", "null"],
+"required" : false</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="184">
   <si>
     <t>color</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Anchors</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Character Classes</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>title</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>desc-en</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>desc-ja</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Character classes can be used in ranges.</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>POSIX Character Classes</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>0000FF</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>POSIX Character Classes must be used in bracket expressions, e.g. [a-z[:upper:]].</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Groups</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>0f000f</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Bracket Expressions</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>000f0f</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Quantifiers</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>0f0f0f</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Special Characters</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>0f00ff</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Assertions</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>00ff0f</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Back References</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Case Modifiers</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Modifiers</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Back references are used in replacements.</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Case modifiers are used in replacements.</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Modifiers can be grouped together, e.g. (?ixm).</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>sign</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>f00000</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>ff0000</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>^</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>$</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>\\A</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>\A</t>
-  </si>
-  <si>
-    <t>\\z</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>\\b</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>\\B</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Matches at the start of string or start of line if multi-line mode is enabled. Many regex implementations have multi-line mode enabled by default.</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Matches at the end of string or end of line if multi-line mode is  enabled. Many regex implementations have multi-line mode enabled by default.</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Matches at the start of the search string.</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Matches at the end of the search string, or before a newline at the end of the string.</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Matches at the end of the search string.</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Matches at word boundaries.</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Matches anywhere but word boundaries.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>\\Z</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>\x{ffff}</t>
-  </si>
-  <si>
-    <t>\s</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>.</t>
@@ -401,33 +1023,15 @@
     <t>Matches white space characters.</t>
   </si>
   <si>
-    <t>\S</t>
-  </si>
-  <si>
     <t>Matches anything but white space characters.</t>
   </si>
   <si>
-    <t>\d</t>
-  </si>
-  <si>
     <t>Matches digits. Equivalent to [0-9].</t>
   </si>
   <si>
-    <t>\D</t>
-  </si>
-  <si>
     <t>Matches anything but digits. Equivalent to [^0-9].</t>
   </si>
   <si>
-    <t>\w</t>
-  </si>
-  <si>
-    <t>\W</t>
-  </si>
-  <si>
-    <t>\xff</t>
-  </si>
-  <si>
     <t>Matches ASCII hexadecimal character ff.</t>
   </si>
   <si>
@@ -440,16 +1044,12 @@
     <t>Matches ASCII octal character 132.</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Matches letters, digits and underscores. Equivalent to [A-Za-z0-9_].</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Matches anything but letters, digits and underscores.</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>[:upper:]</t>
@@ -516,31 +1116,31 @@
   </si>
   <si>
     <t>Matches ASCII characters. Equivalent to \\x00-\\x7f.</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Matches letters, digits and underscores. Equivalent to \\w.</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Matches space and tab. Equivalent to [ \\t].</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Matches space, tab and newline. Equivalent to \\s.</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Matches control characters. Equivalent to [\\x00-\\x1F\\x7F].</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Matches printed characters. Equivalent to [\\x21-\\x7E].</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Matches printed characters and spaces. Equivalent to [\\x21-\\x7E].</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>(foo|bar)</t>
@@ -558,9 +1158,6 @@
     <t>(?&lt;foo&gt;bar)</t>
   </si>
   <si>
-    <t>Define a named group named "foo" consisting of pattern bar. Matches within the group can be referenced in a replacement using the backreference $foo.</t>
-  </si>
-  <si>
     <t>(?:foo)</t>
   </si>
   <si>
@@ -568,11 +1165,11 @@
   </si>
   <si>
     <t>(?&gt;foo+)bar</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Define an atomic group consisting of pattern foo+. Once foo+ has been matched, the regex engine will not try to find other variable length matches of foo+ in order to find a match followed by a maßtch of bar. Atomic groups may be used for perforamce reasons.</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>[adf]</t>
@@ -665,33 +1262,18 @@
     <t>Two, three or four, lazy. Matches will be as small as possible.</t>
   </si>
   <si>
-    <t xml:space="preserve">\\ </t>
-  </si>
-  <si>
     <t>Escape character.</t>
   </si>
   <si>
-    <t>\\n</t>
-  </si>
-  <si>
     <t>Matches newline.</t>
   </si>
   <si>
-    <t>\\t</t>
-  </si>
-  <si>
     <t>Matches tab.</t>
   </si>
   <si>
-    <t>\\r</t>
-  </si>
-  <si>
     <t>Matches carriage return.</t>
   </si>
   <si>
-    <t>\\v</t>
-  </si>
-  <si>
     <t>Matches form feed/page break.</t>
   </si>
   <si>
@@ -732,28 +1314,16 @@
   </si>
   <si>
     <t>$foo</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>\\\u</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Make the next character in the replacement uppercase.</t>
   </si>
   <si>
-    <t>\\\l</t>
-  </si>
-  <si>
     <t>Make the next character in the replacement lowercase.</t>
   </si>
   <si>
-    <t>\\\U</t>
-  </si>
-  <si>
     <t>Make the remaining characters in the replacement uppercase.</t>
-  </si>
-  <si>
-    <t>\\\L</t>
   </si>
   <si>
     <t>Make the remaining characters in the replacement lowercase.</t>
@@ -791,66 +1361,169 @@
     <rPh sb="58" eb="59">
       <t>ハリツケル</t>
     </rPh>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>items</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>sheet://items-Anchors</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>sheet://items-CharClass</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>sheet://items-POSIX-CHAR</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>sheet://items-Groups</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>sheet://items-bracketEx</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>sheet://items-Quantifiers</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>sheet://items-spchar</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>sheet://items-assertion</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>sheet://items-Case Modifiers</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>sheet://items-Modifiers</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>000000</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>\s</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>\S</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>\\\L</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>\A</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>\Z</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>\z</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>\b</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>\B</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>\d</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>\D</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>\w</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>\W</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>\xff</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>\x{ffff}</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>\132</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>\</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>\n</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>\t</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>\r</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>\v</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>\\\u</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>\\\l</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>\\\U</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Define a named group named {foo} consisting of pattern bar. Matches within the group can be referenced in a replacement using the backreference foo.</t>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="6" formatCode="&quot;¥&quot;#,##0;[Red]&quot;¥&quot;\-#,##0"/>
+  <numFmts count="1">
     <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Yu Gothic"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -883,13 +1556,6 @@
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Yu Gothic (本文)"/>
-      <family val="3"/>
-      <charset val="128"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1008,39 +1674,51 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="21" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="21" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="6" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="24" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="21"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="21"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1069,8 +1747,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="21" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="37">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -1093,6 +1772,21 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="36" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1379,65 +2073,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="150" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="11"/>
+      <c r="A1" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="14"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="14"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="14"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="14"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="11"/>
     </row>
     <row r="6" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="14"/>
     </row>
     <row r="7" spans="1:4" ht="21" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D6"/>
   </mergeCells>
-  <phoneticPr fontId="1"/>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:C5"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B1" t="s">
@@ -1449,55 +2143,56 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1"/>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C4"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B1" t="s">
@@ -1508,48 +2203,49 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="6">
+      <c r="A2" s="3">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>151</v>
+      <c r="B2" s="2" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>153</v>
+      <c r="A3" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>155</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>154</v>
+        <v>134</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1"/>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:C5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B1" t="s">
@@ -1561,26 +2257,26 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>156</v>
+        <v>180</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>160</v>
+        <v>182</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1588,26 +2284,29 @@
         <v>162</v>
       </c>
       <c r="B5" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1"/>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B1" t="s">
@@ -1619,40 +2318,41 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
       <c r="B2" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>141</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="B4" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="B5" t="s">
-        <v>171</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1"/>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1661,7 +2361,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
@@ -1683,7 +2383,7 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1693,8 +2393,8 @@
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>174</v>
+      <c r="E2" s="5" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1707,8 +2407,8 @@
       <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>175</v>
+      <c r="E3" s="5" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1721,8 +2421,8 @@
       <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>176</v>
+      <c r="E4" s="5" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1732,8 +2432,8 @@
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>177</v>
+      <c r="E5" s="5" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1743,8 +2443,8 @@
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>178</v>
+      <c r="E6" s="5" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1754,8 +2454,8 @@
       <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>179</v>
+      <c r="E7" s="5" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1765,8 +2465,8 @@
       <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>180</v>
+      <c r="E8" s="5" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1776,13 +2476,13 @@
       <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>181</v>
+      <c r="E9" s="5" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
@@ -1790,13 +2490,13 @@
       <c r="D10" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>181</v>
+      <c r="E10" s="5" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
@@ -1804,13 +2504,13 @@
       <c r="D11" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>182</v>
+      <c r="E11" s="5" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="B12" t="s">
         <v>22</v>
@@ -1818,15 +2518,15 @@
       <c r="D12" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>183</v>
+      <c r="E12" s="5" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E13" s="7"/>
+      <c r="E13" s="4"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="1"/>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
@@ -1840,8 +2540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
@@ -1865,7 +2565,7 @@
         <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1873,209 +2573,69 @@
         <v>30</v>
       </c>
       <c r="C3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>165</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" t="s">
-        <v>42</v>
-      </c>
-    </row>
   </sheetData>
-  <phoneticPr fontId="1"/>
-  <hyperlinks>
-    <hyperlink ref="A5" r:id="rId1"/>
-    <hyperlink ref="A6" r:id="rId2"/>
-    <hyperlink ref="A7" r:id="rId3"/>
-    <hyperlink ref="A8" r:id="rId4"/>
-  </hyperlinks>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <legacyDrawing r:id="rId5"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
-        <v>132</v>
-      </c>
-      <c r="C12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B1" t="s">
@@ -2086,136 +2646,128 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>65</v>
+      <c r="A2" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>160</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>161</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>168</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>169</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>170</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>171</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>172</v>
       </c>
       <c r="B9" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>173</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>163</v>
       </c>
       <c r="B11" t="s">
-        <v>88</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>82</v>
+      <c r="A12" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B13" t="s">
-        <v>90</v>
-      </c>
+      <c r="A13" s="2"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" t="s">
-        <v>91</v>
-      </c>
+      <c r="A14" s="2"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>85</v>
-      </c>
-      <c r="B15" t="s">
-        <v>92</v>
-      </c>
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="1"/>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="A12" numberStoredAsText="1"/>
+  </ignoredErrors>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C6"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B1" t="s">
@@ -2227,63 +2779,136 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>102</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1"/>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="A1:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B1" t="s">
@@ -2295,63 +2920,64 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1"/>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:C11"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B1" t="s">
@@ -2363,103 +2989,64 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="B6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>123</v>
-      </c>
-      <c r="B7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>125</v>
-      </c>
-      <c r="B8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>127</v>
-      </c>
-      <c r="B9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>131</v>
-      </c>
-      <c r="B11" t="s">
-        <v>132</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1"/>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:C6"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B1" t="s">
@@ -2471,47 +3058,157 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>138</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>140</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>141</v>
+        <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>142</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1"/>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>